<commit_message>
Biome, block, drink temperature data
</commit_message>
<xml_diff>
--- a/src/datagen/resources/data/frostedheart/data/drink_temperature.xlsx
+++ b/src/datagen/resources/data/frostedheart/data/drink_temperature.xlsx
@@ -1,38 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\eclipse-workspace\frostedheart-newdev\src\datagen\resources\data\frostedheart\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789B7D14-05F1-4A88-94E1-03A032C63606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16740" yWindow="4110" windowWidth="21420" windowHeight="10155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="drink_temperature" sheetId="1" r:id="rId1"/>
+    <sheet name="drink_temperature" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+  <si>
+    <t/>
+  </si>
   <si>
     <t>fluid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>heat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>caupona:nail_soup</t>
   </si>
   <si>
     <t>minecraft:lava</t>
@@ -44,51 +36,174 @@
     <t>frostedheart:wolfberry_tea</t>
   </si>
   <si>
-    <t>caupona:nail_soup</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>caupona:acquacotta</t>
+  </si>
+  <si>
+    <t>caupona:bisque</t>
+  </si>
+  <si>
+    <t>caupona:borscht</t>
+  </si>
+  <si>
+    <t>caupona:borscht_cream</t>
+  </si>
+  <si>
+    <t>caupona:congee</t>
+  </si>
+  <si>
+    <t>caupona:cream_of_mushroom_soup</t>
+  </si>
+  <si>
+    <t>caupona:cream_of_meat_soup</t>
+  </si>
+  <si>
+    <t>caupona:custard</t>
+  </si>
+  <si>
+    <t>caupona:dilute_soup</t>
+  </si>
+  <si>
+    <t>caupona:egg_drop_soup</t>
+  </si>
+  <si>
+    <t>caupona:egg_tongsui</t>
+  </si>
+  <si>
+    <t>caupona:fish_chowder</t>
+  </si>
+  <si>
+    <t>caupona:fish_soup</t>
+  </si>
+  <si>
+    <t>caupona:fricassee</t>
+  </si>
+  <si>
+    <t>caupona:goji_tongsui</t>
+  </si>
+  <si>
+    <t>caupona:goulash</t>
+  </si>
+  <si>
+    <t>caupona:gruel</t>
+  </si>
+  <si>
+    <t>caupona:hodgepodge</t>
+  </si>
+  <si>
+    <t>caupona:meat_soup</t>
+  </si>
+  <si>
+    <t>caupona:mushroom_soup</t>
+  </si>
+  <si>
+    <t>caupona:nettle_soup</t>
+  </si>
+  <si>
+    <t>caupona:okroshka</t>
+  </si>
+  <si>
+    <t>caupona:porridge</t>
+  </si>
+  <si>
+    <t>caupona:poultry_soup</t>
+  </si>
+  <si>
+    <t>caupona:pumpkin_soup</t>
+  </si>
+  <si>
+    <t>caupona:pumpkin_soup_cream</t>
+  </si>
+  <si>
+    <t>caupona:rice_pudding</t>
+  </si>
+  <si>
+    <t>caupona:scalded_milk</t>
+  </si>
+  <si>
+    <t>caupona:seaweed_soup</t>
+  </si>
+  <si>
+    <t>caupona:stock</t>
+  </si>
+  <si>
+    <t>caupona:stracciatella</t>
+  </si>
+  <si>
+    <t>caupona:ukha</t>
+  </si>
+  <si>
+    <t>caupona:vegetable_chowder</t>
+  </si>
+  <si>
+    <t>caupona:vegetable_soup</t>
+  </si>
+  <si>
+    <t>caupona:walnut_soup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="300" formatCode="General"/>
+  </numFmts>
+  <fonts count="6">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <color rgb="FF175CEB"/>
+      <sz val="10"/>
+      <u/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <name val="Segoe UI Symbol"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="10"/>
-      <color theme="1"/>
+    </font>
+    <font>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -96,28 +211,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0"/>
+    <xf numFmtId="300" fontId="3" fillId="2" borderId="2" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -239,7 +368,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -263,9 +392,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -289,7 +418,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -324,7 +453,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="false">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -342,7 +471,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -367,7 +496,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -375,69 +504,344 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}"/>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr/>
+  <dimension ref="C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView showGridLines="true" tabSelected="true" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="23.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1"/>
+    <col min="1" max="1" width="31.6523" style="9" customWidth="true"/>
+    <col min="2" max="2" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4">
+        <v>114514</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>114514</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.4</v>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="6">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>